<commit_message>
homogenization of data cohort and add FED3 data
</commit_message>
<xml_diff>
--- a/scripts/slope_compilation_v1.xlsx
+++ b/scripts/slope_compilation_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carosandovalcab/Documents/GitHub/data/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE399141-B141-F344-95B6-06F70309F925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3D03B7-31FE-4148-8B87-F5B156489329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="3600" windowWidth="28040" windowHeight="17440" xr2:uid="{D6184119-E9AE-4443-BA5F-733950D4674C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{D6184119-E9AE-4443-BA5F-733950D4674C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="7">
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>BW_SLOPE_LM</t>
   </si>
   <si>
     <t>BW_TIME_INDIVIDUAL_COEFF_LMER</t>
@@ -60,9 +57,6 @@
     <t>NZO/HlLtJ</t>
   </si>
   <si>
-    <t>cumsumFI_SLOPE_LM</t>
-  </si>
-  <si>
     <t>cumsumFI_TIME_INDIVIDUAL_COEFF_LMER</t>
   </si>
 </sst>
@@ -71,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -112,7 +106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,44 +441,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B436B04A-54BD-D44A-9E4C-832EECAC5A01}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>7860</v>
       </c>
@@ -492,22 +478,16 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2">
-        <v>0.1083407714796045</v>
-      </c>
-      <c r="E2" s="2">
-        <v>5.1368360500053187</v>
-      </c>
-      <c r="F2" s="2">
         <v>4.5819205050803964</v>
       </c>
-      <c r="G2" s="3">
+      <c r="E2" s="3">
         <v>283.25659870092522</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7861</v>
       </c>
@@ -515,22 +495,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="2">
-        <v>9.1233174925660285E-2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>5.0735449597322182</v>
-      </c>
-      <c r="F3" s="2">
         <v>3.8763685973003819</v>
       </c>
-      <c r="G3" s="3">
+      <c r="E3" s="3">
         <v>279.7295005981299</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>7862</v>
       </c>
@@ -538,22 +512,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2">
-        <v>8.1356333342518808E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5.4628721954361259</v>
-      </c>
-      <c r="F4" s="2">
         <v>3.4555688812222631</v>
       </c>
-      <c r="G4" s="3">
+      <c r="E4" s="3">
         <v>301.2974885745918</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>7863</v>
       </c>
@@ -561,22 +529,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2">
-        <v>6.1517012332751288E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4.8697092846338386</v>
-      </c>
-      <c r="F5" s="2">
         <v>2.7740652491572781</v>
       </c>
-      <c r="G5" s="3">
+      <c r="E5" s="3">
         <v>268.47284445834839</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>7864</v>
       </c>
@@ -584,22 +546,16 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2">
-        <v>6.3291075978065076E-2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5.2110626206851736</v>
-      </c>
-      <c r="F6" s="2">
         <v>2.8122519051484738</v>
       </c>
-      <c r="G6" s="3">
+      <c r="E6" s="3">
         <v>287.25981034560709</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7865</v>
       </c>
@@ -607,22 +563,16 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2">
-        <v>0.13622693089099919</v>
-      </c>
-      <c r="E7" s="2">
-        <v>6.1739792836589027</v>
-      </c>
-      <c r="F7" s="2">
         <v>5.8358116537524127</v>
       </c>
-      <c r="G7" s="3">
+      <c r="E7" s="3">
         <v>340.68482374890237</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7866</v>
       </c>
@@ -630,22 +580,16 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="2">
-        <v>8.7849622101252231E-2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>4.9868290616395479</v>
-      </c>
-      <c r="F8" s="2">
         <v>3.5324912508435071</v>
       </c>
-      <c r="G8" s="3">
+      <c r="E8" s="3">
         <v>274.87309781700429</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7867</v>
       </c>
@@ -653,22 +597,16 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="2">
-        <v>9.4665339783206126E-2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>4.8790226546897326</v>
-      </c>
-      <c r="F9" s="2">
         <v>3.9141962301637152</v>
       </c>
-      <c r="G9" s="3">
+      <c r="E9" s="3">
         <v>268.95011816683842</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7868</v>
       </c>
@@ -676,22 +614,16 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2">
-        <v>2.6711873811629299E-2</v>
-      </c>
-      <c r="E10" s="2">
-        <v>4.0736146780940921</v>
-      </c>
-      <c r="F10" s="2">
         <v>1.174080634910422</v>
       </c>
-      <c r="G10" s="3">
+      <c r="E10" s="3">
         <v>224.5745335259659</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7869</v>
       </c>
@@ -699,22 +631,16 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2">
-        <v>4.5548472998464332E-2</v>
-      </c>
-      <c r="E11" s="2">
-        <v>4.4969284920409862</v>
-      </c>
-      <c r="F11" s="2">
         <v>1.9392999373594491</v>
       </c>
-      <c r="G11" s="3">
+      <c r="E11" s="3">
         <v>247.89286765320099</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>7870</v>
       </c>
@@ -722,22 +648,16 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2">
-        <v>2.8808785989313059E-2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>4.2566990043842567</v>
-      </c>
-      <c r="F12" s="2">
         <v>1.1350827678600151</v>
       </c>
-      <c r="G12" s="3">
+      <c r="E12" s="3">
         <v>234.57000587322091</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>7871</v>
       </c>
@@ -745,22 +665,16 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2">
-        <v>7.2846785042374185E-2</v>
-      </c>
-      <c r="E13" s="2">
-        <v>5.2299234663972296</v>
-      </c>
-      <c r="F13" s="2">
         <v>3.1987563638960839</v>
       </c>
-      <c r="G13" s="3">
+      <c r="E13" s="3">
         <v>288.32627114679849</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7872</v>
       </c>
@@ -768,22 +682,16 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="2">
-        <v>2.041420428631549E-2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3.8947746712583911</v>
-      </c>
-      <c r="F14" s="2">
         <v>0.89184173504908548</v>
       </c>
-      <c r="G14" s="3">
+      <c r="E14" s="3">
         <v>214.74774419172681</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7873</v>
       </c>
@@ -791,22 +699,16 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="2">
-        <v>4.9622339780947149E-2</v>
-      </c>
-      <c r="E15" s="2">
-        <v>4.7820068853996229</v>
-      </c>
-      <c r="F15" s="2">
         <v>2.1147272770357208</v>
       </c>
-      <c r="G15" s="3">
+      <c r="E15" s="3">
         <v>263.77645306583793</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>7874</v>
       </c>
@@ -814,22 +716,16 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2">
-        <v>3.9046320145065809E-2</v>
-      </c>
-      <c r="E16" s="2">
-        <v>4.3440742140007984</v>
-      </c>
-      <c r="F16" s="2">
         <v>1.6734969540500571</v>
       </c>
-      <c r="G16" s="3">
+      <c r="E16" s="3">
         <v>239.49850508072959</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>7875</v>
       </c>
@@ -837,22 +733,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="2">
-        <v>4.1864804465724409E-2</v>
-      </c>
-      <c r="E17" s="2">
-        <v>4.8812199731692747</v>
-      </c>
-      <c r="F17" s="2">
         <v>1.8050854473170841</v>
       </c>
-      <c r="G17" s="3">
+      <c r="E17" s="3">
         <v>269.22587818840162</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>7876</v>
       </c>
@@ -860,22 +750,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="2">
-        <v>3.6264489504542113E-2</v>
-      </c>
-      <c r="E18" s="2">
-        <v>4.5077357966962142</v>
-      </c>
-      <c r="F18" s="2">
         <v>1.531307452612261</v>
       </c>
-      <c r="G18" s="3">
+      <c r="E18" s="3">
         <v>248.59312163029401</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>7877</v>
       </c>
@@ -883,22 +767,16 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2">
-        <v>5.3338580144228563E-2</v>
-      </c>
-      <c r="E19" s="2">
-        <v>4.8625747102003354</v>
-      </c>
-      <c r="F19" s="2">
         <v>2.2846557700404442</v>
       </c>
-      <c r="G19" s="3">
+      <c r="E19" s="3">
         <v>268.14045970942681</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7878</v>
       </c>
@@ -906,22 +784,16 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="2">
-        <v>2.4806979198568741E-2</v>
-      </c>
-      <c r="E20" s="2">
-        <v>4.3243156889598886</v>
-      </c>
-      <c r="F20" s="2">
         <v>1.105938524539585</v>
       </c>
-      <c r="G20" s="3">
+      <c r="E20" s="3">
         <v>238.45566561786791</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7879</v>
       </c>
@@ -929,22 +801,16 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="2">
-        <v>3.067071781572852E-2</v>
-      </c>
-      <c r="E21" s="2">
-        <v>4.4915758897971703</v>
-      </c>
-      <c r="F21" s="2">
         <v>1.3579190311651419</v>
       </c>
-      <c r="G21" s="3">
+      <c r="E21" s="3">
         <v>247.77141526420979</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7880</v>
       </c>
@@ -952,22 +818,16 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2">
-        <v>1.6814139450524939E-2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>3.964420826095179</v>
-      </c>
-      <c r="F22" s="2">
         <v>0.79052390847682785</v>
       </c>
-      <c r="G22" s="3">
+      <c r="E22" s="3">
         <v>218.6549211418469</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>7881</v>
       </c>
@@ -975,22 +835,16 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="2">
-        <v>1.8149191720046781E-2</v>
-      </c>
-      <c r="E23" s="2">
-        <v>4.0709305074981401</v>
-      </c>
-      <c r="F23" s="2">
         <v>0.87870243021371897</v>
       </c>
-      <c r="G23" s="3">
+      <c r="E23" s="3">
         <v>224.5385986925391</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7882</v>
       </c>
@@ -998,22 +852,16 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="2">
-        <v>2.7191725057054288E-2</v>
-      </c>
-      <c r="E24" s="2">
-        <v>4.2019734223774252</v>
-      </c>
-      <c r="F24" s="2">
         <v>1.199810742665357</v>
       </c>
-      <c r="G24" s="3">
+      <c r="E24" s="3">
         <v>231.7393651650481</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7883</v>
       </c>
@@ -1021,22 +869,16 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="2">
-        <v>8.9423532182142714E-3</v>
-      </c>
-      <c r="E25" s="2">
-        <v>3.9914020786802351</v>
-      </c>
-      <c r="F25" s="2">
         <v>0.48603528839129551</v>
       </c>
-      <c r="G25" s="3">
+      <c r="E25" s="3">
         <v>220.12323230135769</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>3706</v>
       </c>
@@ -1044,22 +886,16 @@
         <v>3</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="2">
-        <v>0.1009320320502675</v>
-      </c>
-      <c r="E26" s="2">
-        <v>5.8048691303167113</v>
-      </c>
-      <c r="F26" s="2">
         <v>3.980483194151764</v>
       </c>
-      <c r="G26" s="3">
+      <c r="E26" s="3">
         <v>320.75368976460481</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>3707</v>
       </c>
@@ -1067,22 +903,16 @@
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="2">
-        <v>0.16297091624383939</v>
-      </c>
-      <c r="E27" s="2">
-        <v>7.0464640249159816</v>
-      </c>
-      <c r="F27" s="2">
         <v>6.7951864624426062</v>
       </c>
-      <c r="G27" s="3">
+      <c r="E27" s="3">
         <v>389.46708257710048</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>3708</v>
       </c>
@@ -1090,22 +920,16 @@
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="2">
-        <v>0.13856926426732449</v>
-      </c>
-      <c r="E28" s="2">
-        <v>6.5450666201623733</v>
-      </c>
-      <c r="F28" s="2">
         <v>5.931245772444262</v>
       </c>
-      <c r="G28" s="3">
+      <c r="E28" s="3">
         <v>361.2690371832137</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>3709</v>
       </c>
@@ -1113,22 +937,16 @@
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29" s="2">
-        <v>0.10938628010805319</v>
-      </c>
-      <c r="E29" s="2">
-        <v>6.2951592891815782</v>
-      </c>
-      <c r="F29" s="2">
         <v>4.6813759236132633</v>
       </c>
-      <c r="G29" s="3">
+      <c r="E29" s="3">
         <v>347.30997379565792</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3710</v>
       </c>
@@ -1136,22 +954,16 @@
         <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30" s="2">
-        <v>0.19156367339614</v>
-      </c>
-      <c r="E30" s="2">
-        <v>6.8144935222670622</v>
-      </c>
-      <c r="F30" s="2">
         <v>7.9682664627454294</v>
       </c>
-      <c r="G30" s="3">
+      <c r="E30" s="3">
         <v>376.25723710030297</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>3711</v>
       </c>
@@ -1159,22 +971,16 @@
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31" s="2">
-        <v>0.13514558801131271</v>
-      </c>
-      <c r="E31" s="2">
-        <v>6.1396190199938934</v>
-      </c>
-      <c r="F31" s="2">
         <v>5.7189664789339201</v>
       </c>
-      <c r="G31" s="3">
+      <c r="E31" s="3">
         <v>338.69350327069441</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3712</v>
       </c>
@@ -1182,22 +988,16 @@
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" s="2">
-        <v>0.12756167705443361</v>
-      </c>
-      <c r="E32" s="2">
-        <v>6.6285358608803273</v>
-      </c>
-      <c r="F32" s="2">
         <v>5.6607747202327339</v>
       </c>
-      <c r="G32" s="3">
+      <c r="E32" s="3">
         <v>366.72428272493369</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>3713</v>
       </c>
@@ -1205,22 +1005,16 @@
         <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33" s="2">
-        <v>9.8562353186931712E-2</v>
-      </c>
-      <c r="E33" s="2">
-        <v>5.9109409442058016</v>
-      </c>
-      <c r="F33" s="2">
         <v>4.1964792316309616</v>
       </c>
-      <c r="G33" s="3">
+      <c r="E33" s="3">
         <v>326.26424124542768</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3714</v>
       </c>
@@ -1228,22 +1022,16 @@
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34" s="2">
-        <v>0.12196635014884689</v>
-      </c>
-      <c r="E34" s="2">
-        <v>5.9912078270636329</v>
-      </c>
-      <c r="F34" s="2">
         <v>5.2768466153769351</v>
       </c>
-      <c r="G34" s="3">
+      <c r="E34" s="3">
         <v>330.48965251041909</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>3716</v>
       </c>
@@ -1251,22 +1039,16 @@
         <v>3</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35" s="2">
-        <v>0.120446560711303</v>
-      </c>
-      <c r="E35" s="2">
-        <v>5.7928912300255924</v>
-      </c>
-      <c r="F35" s="2">
         <v>4.9138921998202569</v>
       </c>
-      <c r="G35" s="3">
+      <c r="E35" s="3">
         <v>320.00350620994328</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>3717</v>
       </c>
@@ -1274,22 +1056,16 @@
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36" s="2">
-        <v>9.9415275452752111E-2</v>
-      </c>
-      <c r="E36" s="2">
-        <v>5.8506738462060586</v>
-      </c>
-      <c r="F36" s="2">
         <v>4.1800756433876582</v>
       </c>
-      <c r="G36" s="3">
+      <c r="E36" s="3">
         <v>323.59110078811739</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>3718</v>
       </c>
@@ -1297,22 +1073,16 @@
         <v>4</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37" s="2">
-        <v>0.1108006957226077</v>
-      </c>
-      <c r="E37" s="2">
-        <v>5.5352287370471229</v>
-      </c>
-      <c r="F37" s="2">
         <v>4.7717146492228864</v>
       </c>
-      <c r="G37" s="3">
+      <c r="E37" s="3">
         <v>305.24642662952948</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>3719</v>
       </c>
@@ -1320,22 +1090,16 @@
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38" s="2">
-        <v>0.1140273805175973</v>
-      </c>
-      <c r="E38" s="2">
-        <v>5.4604892755104828</v>
-      </c>
-      <c r="F38" s="2">
         <v>4.912846547154972</v>
       </c>
-      <c r="G38" s="3">
+      <c r="E38" s="3">
         <v>301.27186696656469</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>3720</v>
       </c>
@@ -1343,22 +1107,16 @@
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39" s="2">
-        <v>7.2540763505380676E-2</v>
-      </c>
-      <c r="E39" s="2">
-        <v>5.3197166428602776</v>
-      </c>
-      <c r="F39" s="2">
         <v>2.815448830062389</v>
       </c>
-      <c r="G39" s="3">
+      <c r="E39" s="3">
         <v>294.01556107067648</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>3721</v>
       </c>
@@ -1366,22 +1124,16 @@
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" s="2">
-        <v>0.1025182030426664</v>
-      </c>
-      <c r="E40" s="2">
-        <v>5.8287199454684862</v>
-      </c>
-      <c r="F40" s="2">
         <v>4.3743390361342556</v>
       </c>
-      <c r="G40" s="3">
+      <c r="E40" s="3">
         <v>321.34145542300462</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>3722</v>
       </c>
@@ -1389,22 +1141,16 @@
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41" s="2">
-        <v>9.0828214887134578E-2</v>
-      </c>
-      <c r="E41" s="2">
-        <v>5.9156956010181201</v>
-      </c>
-      <c r="F41" s="2">
         <v>3.9146017992920199</v>
       </c>
-      <c r="G41" s="3">
+      <c r="E41" s="3">
         <v>326.18240525716072</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3723</v>
       </c>
@@ -1412,22 +1158,16 @@
         <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42" s="2">
-        <v>0.10146370410954331</v>
-      </c>
-      <c r="E42" s="2">
-        <v>6.005091173542362</v>
-      </c>
-      <c r="F42" s="2">
         <v>4.5425227338010874</v>
       </c>
-      <c r="G42" s="3">
+      <c r="E42" s="3">
         <v>331.38951851313942</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>3724</v>
       </c>
@@ -1435,22 +1175,16 @@
         <v>4</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43" s="2">
-        <v>0.13743272783401089</v>
-      </c>
-      <c r="E43" s="2">
-        <v>5.7562740498473914</v>
-      </c>
-      <c r="F43" s="2">
         <v>5.605016135200759</v>
       </c>
-      <c r="G43" s="3">
+      <c r="E43" s="3">
         <v>317.25851239857673</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>3725</v>
       </c>
@@ -1458,22 +1192,16 @@
         <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D44" s="2">
-        <v>0.14300591269184609</v>
-      </c>
-      <c r="E44" s="2">
-        <v>6.1004153178813176</v>
-      </c>
-      <c r="F44" s="2">
         <v>5.7499446310734008</v>
       </c>
-      <c r="G44" s="3">
+      <c r="E44" s="3">
         <v>336.65380762584931</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>3726</v>
       </c>
@@ -1481,22 +1209,16 @@
         <v>4</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D45" s="2">
-        <v>0.17884214958029249</v>
-      </c>
-      <c r="E45" s="2">
-        <v>6.3958067031940802</v>
-      </c>
-      <c r="F45" s="2">
         <v>7.2333781157177448</v>
       </c>
-      <c r="G45" s="3">
+      <c r="E45" s="3">
         <v>352.45727217233008</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>3727</v>
       </c>
@@ -1504,22 +1226,16 @@
         <v>5</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" s="2">
-        <v>0.1359418661348156</v>
-      </c>
-      <c r="E46" s="2">
-        <v>6.2342274767500561</v>
-      </c>
-      <c r="F46" s="2">
         <v>5.5912673784204081</v>
       </c>
-      <c r="G46" s="3">
+      <c r="E46" s="3">
         <v>344.03313715180269</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>3728</v>
       </c>
@@ -1527,22 +1243,16 @@
         <v>5</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47" s="2">
-        <v>0.15816819538402821</v>
-      </c>
-      <c r="E47" s="2">
-        <v>5.8876227255912807</v>
-      </c>
-      <c r="F47" s="2">
         <v>6.4122788822728456</v>
       </c>
-      <c r="G47" s="3">
+      <c r="E47" s="3">
         <v>324.75932373343159</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>3729</v>
       </c>
@@ -1550,26 +1260,19 @@
         <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48" s="2">
-        <v>0.15594978746081459</v>
-      </c>
-      <c r="E48" s="2">
-        <v>6.3034763404742087</v>
-      </c>
-      <c r="F48" s="2">
         <v>6.6207110389229884</v>
       </c>
-      <c r="G48" s="3">
+      <c r="E48" s="3">
         <v>347.69834805312342</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="E49" s="2"/>
-      <c r="G49" s="3"/>
+      <c r="E49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>